<commit_message>
Added a function to calculate Ppk and added code to get LSL line on the plot
</commit_message>
<xml_diff>
--- a/Dashboard/DragonCC_Cals.xlsx
+++ b/Dashboard/DragonCC_Cals.xlsx
@@ -1475,7 +1475,7 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>USL</t>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -1795,7 +1795,7 @@
   <dimension ref="A1:B483"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>